<commit_message>
updated res map functionality
added new lab_dir lookup from spreadsheet, added a helper function to print the order to the screen.
</commit_message>
<xml_diff>
--- a/data/StormVariables.xlsx
+++ b/data/StormVariables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bcrary\Desktop\Projects\RNERRS2\SWMPrStorm\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7471024F-6263-4CB9-B1C3-FFADAFD44469}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DDD4C9B-74CE-43C0-8CDF-B7FC892AB0B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="780" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="780" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MASTER" sheetId="11" r:id="rId1"/>
@@ -23,6 +23,7 @@
     <sheet name="ridgeline" sheetId="7" r:id="rId8"/>
     <sheet name="table_daily" sheetId="10" r:id="rId9"/>
     <sheet name="table_summary" sheetId="12" r:id="rId10"/>
+    <sheet name="reserve_map" sheetId="14" r:id="rId11"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="66">
   <si>
     <t>storm_start</t>
   </si>
@@ -42,9 +43,6 @@
     <t>storm_end</t>
   </si>
   <si>
-    <t>Paramter</t>
-  </si>
-  <si>
     <t>Value</t>
   </si>
   <si>
@@ -99,12 +97,6 @@
     <t>reserve</t>
   </si>
   <si>
-    <t>param</t>
-  </si>
-  <si>
-    <t>value</t>
-  </si>
-  <si>
     <t>flip</t>
   </si>
   <si>
@@ -234,7 +226,13 @@
     <t>2012-11-12 00:00:00</t>
   </si>
   <si>
-    <t>ace, del</t>
+    <t>Comma separated list of reserve label directional orientations (R = right, L = left). The list needs to be the same length as the number of active wq and met stations. The order corresponding to a given station will be printed to the screen in the 01_Generate_Analysis_Results script.</t>
+  </si>
+  <si>
+    <t>lab_dir</t>
+  </si>
+  <si>
+    <t>R, L, L, R, L</t>
   </si>
 </sst>
 </file>
@@ -596,10 +594,10 @@
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -611,35 +609,24 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
         <v>21</v>
-      </c>
-      <c r="B1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C3" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -654,8 +641,8 @@
   </sheetPr>
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -667,24 +654,24 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -692,10 +679,10 @@
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -703,54 +690,108 @@
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>66</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="B5" s="1"/>
       <c r="C5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" t="s">
         <v>35</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C7" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C8" t="s">
-        <v>45</v>
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9413FADA-6183-4A09-B519-B4B46703C9D9}">
+  <sheetPr>
+    <tabColor theme="9"/>
+  </sheetPr>
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -766,7 +807,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -778,13 +819,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
-        <v>3</v>
-      </c>
       <c r="C1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -792,10 +833,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -803,63 +844,63 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B6" s="2" t="b">
         <v>0</v>
       </c>
       <c r="C6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" t="s">
         <v>35</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C7" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C8" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -875,7 +916,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -887,13 +928,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -901,10 +942,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -912,96 +953,96 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C7" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" t="s">
         <v>35</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C10" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C11" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1029,141 +1070,141 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C7" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C8" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" t="s">
         <v>35</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C12" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C13" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1192,110 +1233,110 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C6" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C7" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C8" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B9" s="2" t="b">
         <v>0</v>
       </c>
       <c r="C9" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C10" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1323,13 +1364,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -1337,10 +1378,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -1348,52 +1389,52 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" t="s">
         <v>35</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C6" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C7" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1421,24 +1462,24 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -1446,10 +1487,10 @@
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -1457,61 +1498,61 @@
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" t="s">
         <v>35</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C8" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C9" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1539,24 +1580,24 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -1564,10 +1605,10 @@
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -1575,61 +1616,61 @@
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" t="s">
         <v>35</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C8" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C9" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1645,7 +1686,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="F50" sqref="F50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1657,24 +1698,24 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -1682,10 +1723,10 @@
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -1693,54 +1734,52 @@
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>66</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="B5" s="1"/>
       <c r="C5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" t="s">
         <v>35</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C7" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C8" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>